<commit_message>
added option to run omp or pthread using nonblocked and blocked
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -28,9 +28,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
-    <t>betalgeuse</t>
-  </si>
-  <si>
     <t>class1_omp</t>
   </si>
   <si>
@@ -104,6 +101,9 @@
   </si>
   <si>
     <t>conv5_omp</t>
+  </si>
+  <si>
+    <t>ale</t>
   </si>
 </sst>
 </file>
@@ -436,7 +436,7 @@
   <dimension ref="A2:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,7 +446,7 @@
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -463,127 +463,223 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>40095</v>
+      </c>
+      <c r="C3">
+        <v>57939</v>
+      </c>
+      <c r="D3">
+        <v>138641</v>
+      </c>
+      <c r="E3">
+        <v>11762233</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>31662</v>
+      </c>
+      <c r="C4">
+        <v>93823</v>
+      </c>
+      <c r="D4">
+        <v>116276</v>
+      </c>
+      <c r="E4">
+        <v>4029743</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>46922</v>
+      </c>
+      <c r="C5">
+        <v>101927</v>
+      </c>
+      <c r="D5">
+        <v>128558</v>
+      </c>
+      <c r="E5">
+        <v>15613955</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>38217</v>
+      </c>
+      <c r="C6">
+        <v>71346</v>
+      </c>
+      <c r="D6">
+        <v>90176</v>
+      </c>
+      <c r="E6">
+        <v>4111614</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>375485</v>
+      </c>
+      <c r="C7">
+        <v>495794</v>
+      </c>
+      <c r="D7">
+        <v>434452</v>
+      </c>
+      <c r="E7">
+        <v>4004177</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>4878322</v>
+      </c>
+      <c r="C8">
+        <v>5484645</v>
+      </c>
+      <c r="D8">
+        <v>3629706</v>
+      </c>
+      <c r="E8">
+        <v>7445210</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>47260477</v>
+      </c>
+      <c r="C9">
+        <v>47405558</v>
+      </c>
+      <c r="D9">
+        <v>39485704</v>
+      </c>
+      <c r="E9">
+        <v>35810069</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>358520148</v>
+      </c>
+      <c r="C10">
+        <v>467047849</v>
+      </c>
+      <c r="D10">
+        <v>427695019</v>
+      </c>
+      <c r="E10">
+        <v>381688955</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moved parallel section to outermost loop, classifier_blocked seems buggy
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Dropbox\courses\cs758programming_multicore_processors\cs758workloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\courses\cs758programming_multicore_processors\cs758workloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>class1_omp</t>
   </si>
@@ -104,6 +104,15 @@
   </si>
   <si>
     <t>ale</t>
+  </si>
+  <si>
+    <t>godel omp classifer non-blocked</t>
+  </si>
+  <si>
+    <t>godel omp classifer blocked</t>
+  </si>
+  <si>
+    <t>speedup</t>
   </si>
 </sst>
 </file>
@@ -433,10 +442,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E27"/>
+  <dimension ref="A2:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,7 +453,7 @@
     <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -460,8 +469,11 @@
       <c r="E2">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -478,7 +490,7 @@
         <v>11762233</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -495,7 +507,7 @@
         <v>4029743</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -511,8 +523,12 @@
       <c r="E5">
         <v>15613955</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <f>D5/B5</f>
+        <v>2.7398235369336343</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -528,8 +544,12 @@
       <c r="E6">
         <v>4111614</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <f t="shared" ref="F6:F10" si="0">D6/B6</f>
+        <v>2.359578198184054</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -545,8 +565,12 @@
       <c r="E7">
         <v>4004177</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>1.1570422253884975</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -562,8 +586,15 @@
       <c r="E8">
         <v>7445210</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>0.74404805586839085</v>
+      </c>
+      <c r="H8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -579,8 +610,39 @@
       <c r="E9">
         <v>35810069</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>0.83549101715583618</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="J9">
+        <v>4</v>
+      </c>
+      <c r="K9">
+        <v>8</v>
+      </c>
+      <c r="L9">
+        <v>16</v>
+      </c>
+      <c r="M9">
+        <v>32</v>
+      </c>
+      <c r="N9">
+        <v>64</v>
+      </c>
+      <c r="O9">
+        <v>128</v>
+      </c>
+      <c r="P9">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -596,88 +658,248 @@
       <c r="E10">
         <v>381688955</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>1.1929455607610651</v>
+      </c>
+      <c r="H10">
+        <v>115</v>
+      </c>
+      <c r="I10">
+        <v>71</v>
+      </c>
+      <c r="J10">
+        <v>84</v>
+      </c>
+      <c r="K10">
+        <v>51</v>
+      </c>
+      <c r="L10">
+        <v>52</v>
+      </c>
+      <c r="M10">
+        <v>54</v>
+      </c>
+      <c r="N10">
+        <v>47</v>
+      </c>
+      <c r="O10">
+        <v>34</v>
+      </c>
+      <c r="P10">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <f>$H$10/H10</f>
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <f t="shared" ref="I11:P11" si="1">$H$10/I10</f>
+        <v>1.619718309859155</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>1.3690476190476191</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>2.2549019607843137</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="1"/>
+        <v>2.2115384615384617</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="1"/>
+        <v>2.1296296296296298</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="1"/>
+        <v>2.4468085106382977</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="1"/>
+        <v>3.3823529411764706</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="1"/>
+        <v>2.2549019607843137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+      <c r="J15">
+        <v>4</v>
+      </c>
+      <c r="K15">
+        <v>8</v>
+      </c>
+      <c r="L15">
+        <v>16</v>
+      </c>
+      <c r="M15">
+        <v>32</v>
+      </c>
+      <c r="N15">
+        <v>64</v>
+      </c>
+      <c r="O15">
+        <v>128</v>
+      </c>
+      <c r="P15">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <v>115</v>
+      </c>
+      <c r="I16">
+        <v>69</v>
+      </c>
+      <c r="J16">
+        <v>66</v>
+      </c>
+      <c r="K16">
+        <v>50</v>
+      </c>
+      <c r="L16">
+        <v>52</v>
+      </c>
+      <c r="M16">
+        <v>54</v>
+      </c>
+      <c r="N16">
+        <v>38</v>
+      </c>
+      <c r="O16">
+        <v>35</v>
+      </c>
+      <c r="P16">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <f>$H$16/H16</f>
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <f t="shared" ref="I17:P17" si="2">$H$16/I16</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="2"/>
+        <v>1.7424242424242424</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="2"/>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="2"/>
+        <v>2.2115384615384617</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="2"/>
+        <v>2.1296296296296298</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="2"/>
+        <v>3.0263157894736841</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="2"/>
+        <v>3.2857142857142856</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="2"/>
+        <v>2.1296296296296298</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
fixed bug with omp ime-sad
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -30,6 +30,7 @@
     <definedName name="results" localSheetId="3">'SIFT-DOG pthread'!$A$1:$H$140</definedName>
     <definedName name="results_1" localSheetId="6">'IME-SAD omp'!$A$1:$H$180</definedName>
     <definedName name="results_1" localSheetId="4">'SIFT-DOG omp'!$A$1:$H$180</definedName>
+    <definedName name="results_2" localSheetId="6">'IME-SAD omp'!$A$1:$H$180</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -127,6 +128,20 @@
     </textPr>
   </connection>
   <connection id="7" name="results32" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="\\psf\Dropbox\courses\cs758programming_multicore_processors\cs758workloads\conv-engine\omp\ime-sad\results.txt" space="1" consecutive="1">
+      <textFields count="8">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="8" name="results33" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="437" sourceFile="\\psf\Dropbox\courses\cs758programming_multicore_processors\cs758workloads\conv-engine\omp\ime-sad\results.txt" space="1" consecutive="1">
       <textFields count="8">
         <textField/>
@@ -3032,6 +3047,955 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="5"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>pthread_godel!$L$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>pool1p_pthread</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>pthread_godel!$M$2:$U$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>pthread_godel!$M$11:$U$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5725972526062355</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0415726541381267</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0954182213395414</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.7542067996036752</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.48646258974900208</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.28728737118916592</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.16455058887670584</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.1153820882839812E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>pthread_godel!$L$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>pool3p_pthread</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>pthread_godel!$M$2:$U$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>pthread_godel!$M$12:$U$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.85100089745082863</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.71084975099893699</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.34995052311679714</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.19195849596151551</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.11737253002940934</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.4707854933156922E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.0574629184652351E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.5181182188973956E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>pthread_godel!$L$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>pool5p_pthread</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>pthread_godel!$M$2:$U$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>pthread_godel!$M$13:$U$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8169186778692612</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0568080027572484</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.8733352587757865</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.9121425410085475</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.1912228794791528</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.4365403263600787</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.91960730515589417</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.52963056312905876</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>pthread_godel!$L$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>pool1_pthread</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>pthread_godel!$M$2:$U$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>pthread_godel!$M$14:$U$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6846787813054955</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1931524892660379</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5471354730071165</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.96777788327598369</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.67284286507867008</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.43689786376025463</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.21478265378587938</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.11797037691217005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>pthread_godel!$L$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>pool3_pthread</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>pthread_godel!$M$2:$U$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>pthread_godel!$M$15:$U$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.92597292092731642</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.58753167956852193</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.34966684973691037</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.17967107130650384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.10176550411669717</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.2959782350308821E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.6290224191353549E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.3331917271923921E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>pthread_godel!$L$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>pool5_pthread</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>pthread_godel!$M$2:$U$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>pthread_godel!$M$16:$U$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8976648749554568</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.3254837051502903</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.7899728534173542</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.3570141494246601</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0950387293151644</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.4986612120769729</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.94737263420941853</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.52450092849938834</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>pthread_godel!$L$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>pool6_pthread</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>pthread_godel!$M$2:$U$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>pthread_godel!$M$17:$U$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8669735591512362</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.1820198498321224</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.1413942938785047</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.0070908019339737</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0526572892898787</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.484586621554123</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.93118475999674888</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.531454368290321</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="254012496"/>
+        <c:axId val="254015296"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="254012496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="254015296"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="254015296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="254012496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
@@ -5669,7 +6633,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -6316,7 +7280,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -6963,7 +7927,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -7610,7 +8574,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -8246,7 +9210,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -8369,28 +9333,28 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.83517573520213195</c:v>
+                  <c:v>0.28939195076887475</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.97620971643709331</c:v>
+                  <c:v>0.16927365322144017</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.81103249283302081</c:v>
+                  <c:v>9.3494472427552822E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.97485305691317514</c:v>
+                  <c:v>4.7185845779078181E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.80226940310934336</c:v>
+                  <c:v>2.3395098247837566E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.79726577109052299</c:v>
+                  <c:v>1.2394146174675109E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0074270291070515</c:v>
+                  <c:v>5.0330625259197561E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.95562120636281533</c:v>
+                  <c:v>1.9790186635964243E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8469,28 +9433,28 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.7964411631078725</c:v>
+                  <c:v>1.4883156934744521</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.77363985319213135</c:v>
+                  <c:v>1.6784034318501677</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.81704035384048723</c:v>
+                  <c:v>1.1954484643796217</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.78595908683304361</c:v>
+                  <c:v>0.71656915190175452</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.99378512684997555</c:v>
+                  <c:v>0.36602938450950462</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0164501964759531</c:v>
+                  <c:v>0.18650130048505228</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.98057492398208368</c:v>
+                  <c:v>7.7421306859909333E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.80378251916664567</c:v>
+                  <c:v>3.11698887143145E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8569,28 +9533,28 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.9352289950349828</c:v>
+                  <c:v>1.8703996122442992</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.98970661517945968</c:v>
+                  <c:v>3.2702612603844283</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.97617926032751456</c:v>
+                  <c:v>4.6326751565687081</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.83481752587553881</c:v>
+                  <c:v>4.6081471968184466</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.88132149280393268</c:v>
+                  <c:v>3.1703042933122769</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.81894709694398504</c:v>
+                  <c:v>1.9903845597848957</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.83680334284021685</c:v>
+                  <c:v>1.0522199933564251</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.81717921254936665</c:v>
+                  <c:v>0.46964650684469855</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8669,28 +9633,28 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.98022200796754633</c:v>
+                  <c:v>1.9879401308808013</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.9796409158653665</c:v>
+                  <c:v>3.9420211008206212</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.9793437850008585</c:v>
+                  <c:v>7.614528283848875</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.99377807818181918</c:v>
+                  <c:v>13.571983566287329</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.9663208152678604</c:v>
+                  <c:v>13.861376231815902</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0217056639752791</c:v>
+                  <c:v>12.405226327876129</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.99005493923764887</c:v>
+                  <c:v>8.5548078573289299</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0020469069661928</c:v>
+                  <c:v>4.6014914880416873</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8893,7 +9857,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -9015,28 +9979,28 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.83517573520213195</c:v>
+                  <c:v>0.28939195076887475</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.97620971643709331</c:v>
+                  <c:v>0.16927365322144017</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.81103249283302081</c:v>
+                  <c:v>9.3494472427552822E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.97485305691317514</c:v>
+                  <c:v>4.7185845779078181E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.80226940310934336</c:v>
+                  <c:v>2.3395098247837566E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.79726577109052299</c:v>
+                  <c:v>1.2394146174675109E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0074270291070515</c:v>
+                  <c:v>5.0330625259197561E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.95562120636281533</c:v>
+                  <c:v>1.9790186635964243E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9112,28 +10076,28 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.7964411631078725</c:v>
+                  <c:v>1.4883156934744521</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.77363985319213135</c:v>
+                  <c:v>1.6784034318501677</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.81704035384048723</c:v>
+                  <c:v>1.1954484643796217</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.78595908683304361</c:v>
+                  <c:v>0.71656915190175452</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.99378512684997555</c:v>
+                  <c:v>0.36602938450950462</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0164501964759531</c:v>
+                  <c:v>0.18650130048505228</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.98057492398208368</c:v>
+                  <c:v>7.7421306859909333E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.80378251916664567</c:v>
+                  <c:v>3.11698887143145E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9209,28 +10173,28 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.9352289950349828</c:v>
+                  <c:v>1.8703996122442992</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.98970661517945968</c:v>
+                  <c:v>3.2702612603844283</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.97617926032751456</c:v>
+                  <c:v>4.6326751565687081</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.83481752587553881</c:v>
+                  <c:v>4.6081471968184466</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.88132149280393268</c:v>
+                  <c:v>3.1703042933122769</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.81894709694398504</c:v>
+                  <c:v>1.9903845597848957</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.83680334284021685</c:v>
+                  <c:v>1.0522199933564251</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.81717921254936665</c:v>
+                  <c:v>0.46964650684469855</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9306,28 +10270,28 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.98022200796754633</c:v>
+                  <c:v>1.9879401308808013</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.9796409158653665</c:v>
+                  <c:v>3.9420211008206212</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.9793437850008585</c:v>
+                  <c:v>7.614528283848875</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.99377807818181918</c:v>
+                  <c:v>13.571983566287329</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.9663208152678604</c:v>
+                  <c:v>13.861376231815902</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0217056639752791</c:v>
+                  <c:v>12.405226327876129</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.99005493923764887</c:v>
+                  <c:v>8.5548078573289299</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0020469069661928</c:v>
+                  <c:v>4.6014914880416873</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9810,6 +10774,46 @@
 </file>
 
 <file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -13977,20 +14981,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -14004,6 +15524,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -14447,10 +15997,14 @@
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="results_2" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="results_1" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="results" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -15285,7 +16839,7 @@
   <dimension ref="A2:U26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:U25"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34679,7 +36233,7 @@
   <dimension ref="A1:S180"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection sqref="A1:H180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34721,7 +36275,7 @@
         <v>1</v>
       </c>
       <c r="H1">
-        <v>44246114</v>
+        <v>80059</v>
       </c>
       <c r="K1" t="s">
         <v>57</v>
@@ -34753,7 +36307,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>41545080</v>
+        <v>82546</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -34809,7 +36363,7 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>35406700</v>
+        <v>80038</v>
       </c>
       <c r="I3" t="s">
         <v>58</v>
@@ -34819,39 +36373,39 @@
       </c>
       <c r="K3">
         <f ca="1">MIN(OFFSET($H1,(COLUMN()-11)*5,0,1,1):OFFSET($H1,(COLUMN()+1-11)*5-1,0,1,1))</f>
-        <v>32091722</v>
+        <v>80038</v>
       </c>
       <c r="L3">
         <f ca="1">MIN(OFFSET($H1,(COLUMN()-11)*5,0,1,1):OFFSET($H1,(COLUMN()+1-11)*5-1,0,1,1))</f>
-        <v>38425113</v>
+        <v>276573</v>
       </c>
       <c r="M3">
         <f ca="1">MIN(OFFSET($H1,(COLUMN()-11)*5,0,1,1):OFFSET($H1,(COLUMN()+1-11)*5-1,0,1,1))</f>
-        <v>32873799</v>
+        <v>472832</v>
       </c>
       <c r="N3">
         <f ca="1">MIN(OFFSET($H1,(COLUMN()-11)*5,0,1,1):OFFSET($H1,(COLUMN()+1-11)*5-1,0,1,1))</f>
-        <v>39568972</v>
+        <v>856072</v>
       </c>
       <c r="O3">
         <f ca="1">MIN(OFFSET($H1,(COLUMN()-11)*5,0,1,1):OFFSET($H1,(COLUMN()+1-11)*5-1,0,1,1))</f>
-        <v>32919548</v>
+        <v>1696229</v>
       </c>
       <c r="P3">
         <f ca="1">MIN(OFFSET($H1,(COLUMN()-11)*5,0,1,1):OFFSET($H1,(COLUMN()+1-11)*5-1,0,1,1))</f>
-        <v>40001179</v>
+        <v>3421144</v>
       </c>
       <c r="Q3">
         <f ca="1">MIN(OFFSET($H1,(COLUMN()-11)*5,0,1,1):OFFSET($H1,(COLUMN()+1-11)*5-1,0,1,1))</f>
-        <v>40252226</v>
+        <v>6457726</v>
       </c>
       <c r="R3">
         <f ca="1">MIN(OFFSET($H1,(COLUMN()-11)*5,0,1,1):OFFSET($H1,(COLUMN()+1-11)*5-1,0,1,1))</f>
-        <v>31855133</v>
+        <v>15902445</v>
       </c>
       <c r="S3">
         <f ca="1">MIN(OFFSET($H1,(COLUMN()-11)*5,0,1,1):OFFSET($H1,(COLUMN()+1-11)*5-1,0,1,1))</f>
-        <v>33582053</v>
+        <v>40443277</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -34880,46 +36434,46 @@
         <v>1</v>
       </c>
       <c r="H4">
-        <v>37943205</v>
+        <v>84290</v>
       </c>
       <c r="J4" t="s">
         <v>60</v>
       </c>
       <c r="K4">
         <f ca="1">MIN(OFFSET($H46,(COLUMN()-11)*5,0,1,1):OFFSET($H46,(COLUMN()+1-11)*5-1,0,1,1))</f>
-        <v>31678327</v>
+        <v>1240273</v>
       </c>
       <c r="L4">
         <f ca="1">MIN(OFFSET($H46,(COLUMN()-11)*5,0,1,1):OFFSET($H46,(COLUMN()+1-11)*5-1,0,1,1))</f>
-        <v>39774849</v>
+        <v>833340</v>
       </c>
       <c r="M4">
         <f ca="1">MIN(OFFSET($H46,(COLUMN()-11)*5,0,1,1):OFFSET($H46,(COLUMN()+1-11)*5-1,0,1,1))</f>
-        <v>40947124</v>
+        <v>738960</v>
       </c>
       <c r="N4">
         <f ca="1">MIN(OFFSET($H46,(COLUMN()-11)*5,0,1,1):OFFSET($H46,(COLUMN()+1-11)*5-1,0,1,1))</f>
-        <v>38772047</v>
+        <v>1037496</v>
       </c>
       <c r="O4">
         <f ca="1">MIN(OFFSET($H46,(COLUMN()-11)*5,0,1,1):OFFSET($H46,(COLUMN()+1-11)*5-1,0,1,1))</f>
-        <v>40305313</v>
+        <v>1730849</v>
       </c>
       <c r="P4">
         <f ca="1">MIN(OFFSET($H46,(COLUMN()-11)*5,0,1,1):OFFSET($H46,(COLUMN()+1-11)*5-1,0,1,1))</f>
-        <v>31876435</v>
+        <v>3388452</v>
       </c>
       <c r="Q4">
         <f ca="1">MIN(OFFSET($H46,(COLUMN()-11)*5,0,1,1):OFFSET($H46,(COLUMN()+1-11)*5-1,0,1,1))</f>
-        <v>31165646</v>
+        <v>6650211</v>
       </c>
       <c r="R4">
         <f ca="1">MIN(OFFSET($H46,(COLUMN()-11)*5,0,1,1):OFFSET($H46,(COLUMN()+1-11)*5-1,0,1,1))</f>
-        <v>32305871</v>
+        <v>16019789</v>
       </c>
       <c r="S4">
         <f ca="1">MIN(OFFSET($H46,(COLUMN()-11)*5,0,1,1):OFFSET($H46,(COLUMN()+1-11)*5-1,0,1,1))</f>
-        <v>39411565</v>
+        <v>39790742</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -34948,46 +36502,46 @@
         <v>1</v>
       </c>
       <c r="H5">
-        <v>32091722</v>
+        <v>81364</v>
       </c>
       <c r="J5" t="s">
         <v>61</v>
       </c>
       <c r="K5">
         <f ca="1">MIN(OFFSET($H91,(COLUMN()-11)*5,0,1,1):OFFSET($H91,(COLUMN()+1-11)*5-1,0,1,1))</f>
-        <v>32611407</v>
+        <v>15489720</v>
       </c>
       <c r="L5">
         <f ca="1">MIN(OFFSET($H91,(COLUMN()-11)*5,0,1,1):OFFSET($H91,(COLUMN()+1-11)*5-1,0,1,1))</f>
-        <v>34869970</v>
+        <v>8281503</v>
       </c>
       <c r="M5">
         <f ca="1">MIN(OFFSET($H91,(COLUMN()-11)*5,0,1,1):OFFSET($H91,(COLUMN()+1-11)*5-1,0,1,1))</f>
-        <v>32950580</v>
+        <v>4736539</v>
       </c>
       <c r="N5">
         <f ca="1">MIN(OFFSET($H91,(COLUMN()-11)*5,0,1,1):OFFSET($H91,(COLUMN()+1-11)*5-1,0,1,1))</f>
-        <v>33407191</v>
+        <v>3343580</v>
       </c>
       <c r="O5">
         <f ca="1">MIN(OFFSET($H91,(COLUMN()-11)*5,0,1,1):OFFSET($H91,(COLUMN()+1-11)*5-1,0,1,1))</f>
-        <v>39064114</v>
+        <v>3361377</v>
       </c>
       <c r="P5">
         <f ca="1">MIN(OFFSET($H91,(COLUMN()-11)*5,0,1,1):OFFSET($H91,(COLUMN()+1-11)*5-1,0,1,1))</f>
-        <v>37002850</v>
+        <v>4885878</v>
       </c>
       <c r="Q5">
         <f ca="1">MIN(OFFSET($H91,(COLUMN()-11)*5,0,1,1):OFFSET($H91,(COLUMN()+1-11)*5-1,0,1,1))</f>
-        <v>39821140</v>
+        <v>7782275</v>
       </c>
       <c r="R5">
         <f ca="1">MIN(OFFSET($H91,(COLUMN()-11)*5,0,1,1):OFFSET($H91,(COLUMN()+1-11)*5-1,0,1,1))</f>
-        <v>38971411</v>
+        <v>14720990</v>
       </c>
       <c r="S5">
         <f ca="1">MIN(OFFSET($H91,(COLUMN()-11)*5,0,1,1):OFFSET($H91,(COLUMN()+1-11)*5-1,0,1,1))</f>
-        <v>39907289</v>
+        <v>32981657</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -35016,46 +36570,46 @@
         <v>2</v>
       </c>
       <c r="H6">
-        <v>40591614</v>
+        <v>277511</v>
       </c>
       <c r="J6" t="s">
         <v>62</v>
       </c>
       <c r="K6">
         <f ca="1">MIN(OFFSET($H136,(COLUMN()-11)*5,0,1,1):OFFSET($H136,(COLUMN()+1-11)*5-1,0,1,1))</f>
-        <v>42117745</v>
+        <v>232734600</v>
       </c>
       <c r="L6">
         <f ca="1">MIN(OFFSET($H136,(COLUMN()-11)*5,0,1,1):OFFSET($H136,(COLUMN()+1-11)*5-1,0,1,1))</f>
-        <v>42967557</v>
+        <v>117073244</v>
       </c>
       <c r="M6">
         <f ca="1">MIN(OFFSET($H136,(COLUMN()-11)*5,0,1,1):OFFSET($H136,(COLUMN()+1-11)*5-1,0,1,1))</f>
-        <v>42993044</v>
+        <v>59039410</v>
       </c>
       <c r="N6">
         <f ca="1">MIN(OFFSET($H136,(COLUMN()-11)*5,0,1,1):OFFSET($H136,(COLUMN()+1-11)*5-1,0,1,1))</f>
-        <v>43006088</v>
+        <v>30564546</v>
       </c>
       <c r="O6">
         <f ca="1">MIN(OFFSET($H136,(COLUMN()-11)*5,0,1,1):OFFSET($H136,(COLUMN()+1-11)*5-1,0,1,1))</f>
-        <v>42381439</v>
+        <v>17148164</v>
       </c>
       <c r="P6">
         <f ca="1">MIN(OFFSET($H136,(COLUMN()-11)*5,0,1,1):OFFSET($H136,(COLUMN()+1-11)*5-1,0,1,1))</f>
-        <v>43585675</v>
+        <v>16790151</v>
       </c>
       <c r="Q6">
         <f ca="1">MIN(OFFSET($H136,(COLUMN()-11)*5,0,1,1):OFFSET($H136,(COLUMN()+1-11)*5-1,0,1,1))</f>
-        <v>41222973</v>
+        <v>18761012</v>
       </c>
       <c r="R6">
         <f ca="1">MIN(OFFSET($H136,(COLUMN()-11)*5,0,1,1):OFFSET($H136,(COLUMN()+1-11)*5-1,0,1,1))</f>
-        <v>42540816</v>
+        <v>27205123</v>
       </c>
       <c r="S6">
         <f ca="1">MIN(OFFSET($H136,(COLUMN()-11)*5,0,1,1):OFFSET($H136,(COLUMN()+1-11)*5-1,0,1,1))</f>
-        <v>42031710</v>
+        <v>50578079</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -35084,7 +36638,7 @@
         <v>2</v>
       </c>
       <c r="H7">
-        <v>38425113</v>
+        <v>277867</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -35113,7 +36667,7 @@
         <v>2</v>
       </c>
       <c r="H8">
-        <v>41766690</v>
+        <v>283648</v>
       </c>
       <c r="K8">
         <f>COLUMN()</f>
@@ -35146,7 +36700,7 @@
         <v>2</v>
       </c>
       <c r="H9">
-        <v>40183867</v>
+        <v>276573</v>
       </c>
       <c r="K9">
         <f>ROW()</f>
@@ -35183,7 +36737,7 @@
         <v>2</v>
       </c>
       <c r="H10">
-        <v>41397628</v>
+        <v>328882</v>
       </c>
       <c r="M10" t="e">
         <f ca="1">B(column-5)</f>
@@ -35216,7 +36770,7 @@
         <v>4</v>
       </c>
       <c r="H11">
-        <v>41686756</v>
+        <v>472832</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -35245,7 +36799,7 @@
         <v>4</v>
       </c>
       <c r="H12">
-        <v>41712472</v>
+        <v>482721</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -35274,7 +36828,7 @@
         <v>4</v>
       </c>
       <c r="H13">
-        <v>32873799</v>
+        <v>481864</v>
       </c>
       <c r="K13" t="s">
         <v>63</v>
@@ -35306,7 +36860,7 @@
         <v>4</v>
       </c>
       <c r="H14">
-        <v>40615858</v>
+        <v>490051</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -35335,7 +36889,7 @@
         <v>4</v>
       </c>
       <c r="H15">
-        <v>42743421</v>
+        <v>535794</v>
       </c>
       <c r="K15">
         <f t="shared" ref="K15:S15" si="0">K2</f>
@@ -35400,7 +36954,7 @@
         <v>8</v>
       </c>
       <c r="H16">
-        <v>41048029</v>
+        <v>856072</v>
       </c>
       <c r="J16" t="str">
         <f t="shared" ref="J16:S19" si="1">J3</f>
@@ -35412,35 +36966,35 @@
       </c>
       <c r="L16">
         <f t="shared" ref="L16:S16" ca="1" si="2">$K3/L3</f>
-        <v>0.83517573520213195</v>
+        <v>0.28939195076887475</v>
       </c>
       <c r="M16">
         <f t="shared" ca="1" si="2"/>
-        <v>0.97620971643709331</v>
+        <v>0.16927365322144017</v>
       </c>
       <c r="N16">
         <f t="shared" ca="1" si="2"/>
-        <v>0.81103249283302081</v>
+        <v>9.3494472427552822E-2</v>
       </c>
       <c r="O16">
         <f t="shared" ca="1" si="2"/>
-        <v>0.97485305691317514</v>
+        <v>4.7185845779078181E-2</v>
       </c>
       <c r="P16">
         <f t="shared" ca="1" si="2"/>
-        <v>0.80226940310934336</v>
+        <v>2.3395098247837566E-2</v>
       </c>
       <c r="Q16">
         <f t="shared" ca="1" si="2"/>
-        <v>0.79726577109052299</v>
+        <v>1.2394146174675109E-2</v>
       </c>
       <c r="R16">
         <f t="shared" ca="1" si="2"/>
-        <v>1.0074270291070515</v>
+        <v>5.0330625259197561E-3</v>
       </c>
       <c r="S16">
         <f t="shared" ca="1" si="2"/>
-        <v>0.95562120636281533</v>
+        <v>1.9790186635964243E-3</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
@@ -35469,7 +37023,7 @@
         <v>8</v>
       </c>
       <c r="H17">
-        <v>40103573</v>
+        <v>903957</v>
       </c>
       <c r="J17" t="str">
         <f t="shared" si="1"/>
@@ -35481,35 +37035,35 @@
       </c>
       <c r="L17">
         <f t="shared" ca="1" si="3"/>
-        <v>0.7964411631078725</v>
+        <v>1.4883156934744521</v>
       </c>
       <c r="M17">
         <f t="shared" ca="1" si="3"/>
-        <v>0.77363985319213135</v>
+        <v>1.6784034318501677</v>
       </c>
       <c r="N17">
         <f t="shared" ca="1" si="3"/>
-        <v>0.81704035384048723</v>
+        <v>1.1954484643796217</v>
       </c>
       <c r="O17">
         <f t="shared" ca="1" si="3"/>
-        <v>0.78595908683304361</v>
+        <v>0.71656915190175452</v>
       </c>
       <c r="P17">
         <f t="shared" ca="1" si="3"/>
-        <v>0.99378512684997555</v>
+        <v>0.36602938450950462</v>
       </c>
       <c r="Q17">
         <f t="shared" ca="1" si="3"/>
-        <v>1.0164501964759531</v>
+        <v>0.18650130048505228</v>
       </c>
       <c r="R17">
         <f t="shared" ca="1" si="3"/>
-        <v>0.98057492398208368</v>
+        <v>7.7421306859909333E-2</v>
       </c>
       <c r="S17">
         <f t="shared" ca="1" si="3"/>
-        <v>0.80378251916664567</v>
+        <v>3.11698887143145E-2</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
@@ -35538,7 +37092,7 @@
         <v>8</v>
       </c>
       <c r="H18">
-        <v>40056493</v>
+        <v>928679</v>
       </c>
       <c r="J18" t="str">
         <f t="shared" si="1"/>
@@ -35550,35 +37104,35 @@
       </c>
       <c r="L18">
         <f t="shared" ca="1" si="3"/>
-        <v>0.9352289950349828</v>
+        <v>1.8703996122442992</v>
       </c>
       <c r="M18">
         <f t="shared" ca="1" si="3"/>
-        <v>0.98970661517945968</v>
+        <v>3.2702612603844283</v>
       </c>
       <c r="N18">
         <f t="shared" ca="1" si="3"/>
-        <v>0.97617926032751456</v>
+        <v>4.6326751565687081</v>
       </c>
       <c r="O18">
         <f t="shared" ca="1" si="3"/>
-        <v>0.83481752587553881</v>
+        <v>4.6081471968184466</v>
       </c>
       <c r="P18">
         <f t="shared" ca="1" si="3"/>
-        <v>0.88132149280393268</v>
+        <v>3.1703042933122769</v>
       </c>
       <c r="Q18">
         <f t="shared" ca="1" si="3"/>
-        <v>0.81894709694398504</v>
+        <v>1.9903845597848957</v>
       </c>
       <c r="R18">
         <f t="shared" ca="1" si="3"/>
-        <v>0.83680334284021685</v>
+        <v>1.0522199933564251</v>
       </c>
       <c r="S18">
         <f t="shared" ca="1" si="3"/>
-        <v>0.81717921254936665</v>
+        <v>0.46964650684469855</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
@@ -35607,7 +37161,7 @@
         <v>8</v>
       </c>
       <c r="H19">
-        <v>42071331</v>
+        <v>925366</v>
       </c>
       <c r="J19" t="str">
         <f t="shared" si="1"/>
@@ -35619,35 +37173,35 @@
       </c>
       <c r="L19">
         <f t="shared" ca="1" si="3"/>
-        <v>0.98022200796754633</v>
+        <v>1.9879401308808013</v>
       </c>
       <c r="M19">
         <f t="shared" ca="1" si="3"/>
-        <v>0.9796409158653665</v>
+        <v>3.9420211008206212</v>
       </c>
       <c r="N19">
         <f t="shared" ca="1" si="3"/>
-        <v>0.9793437850008585</v>
+        <v>7.614528283848875</v>
       </c>
       <c r="O19">
         <f t="shared" ca="1" si="3"/>
-        <v>0.99377807818181918</v>
+        <v>13.571983566287329</v>
       </c>
       <c r="P19">
         <f t="shared" ca="1" si="3"/>
-        <v>0.9663208152678604</v>
+        <v>13.861376231815902</v>
       </c>
       <c r="Q19">
         <f t="shared" ca="1" si="3"/>
-        <v>1.0217056639752791</v>
+        <v>12.405226327876129</v>
       </c>
       <c r="R19">
         <f t="shared" ca="1" si="3"/>
-        <v>0.99005493923764887</v>
+        <v>8.5548078573289299</v>
       </c>
       <c r="S19">
         <f t="shared" ca="1" si="3"/>
-        <v>1.0020469069661928</v>
+        <v>4.6014914880416873</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
@@ -35676,7 +37230,7 @@
         <v>8</v>
       </c>
       <c r="H20">
-        <v>39568972</v>
+        <v>912500</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
@@ -35705,7 +37259,7 @@
         <v>16</v>
       </c>
       <c r="H21">
-        <v>41094314</v>
+        <v>1731668</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
@@ -35734,7 +37288,7 @@
         <v>16</v>
       </c>
       <c r="H22">
-        <v>40786904</v>
+        <v>1782693</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
@@ -35763,7 +37317,7 @@
         <v>16</v>
       </c>
       <c r="H23">
-        <v>32919548</v>
+        <v>1853180</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
@@ -35792,7 +37346,7 @@
         <v>16</v>
       </c>
       <c r="H24">
-        <v>47470400</v>
+        <v>1782763</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
@@ -35821,7 +37375,7 @@
         <v>16</v>
       </c>
       <c r="H25">
-        <v>41180607</v>
+        <v>1696229</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
@@ -35850,7 +37404,7 @@
         <v>32</v>
       </c>
       <c r="H26">
-        <v>40001179</v>
+        <v>3446012</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
@@ -35879,7 +37433,7 @@
         <v>32</v>
       </c>
       <c r="H27">
-        <v>48102934</v>
+        <v>3432325</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
@@ -35908,7 +37462,7 @@
         <v>32</v>
       </c>
       <c r="H28">
-        <v>41706180</v>
+        <v>3444058</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
@@ -35937,7 +37491,7 @@
         <v>32</v>
       </c>
       <c r="H29">
-        <v>40823541</v>
+        <v>3539768</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
@@ -35966,7 +37520,7 @@
         <v>32</v>
       </c>
       <c r="H30">
-        <v>41771162</v>
+        <v>3421144</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
@@ -35995,7 +37549,7 @@
         <v>64</v>
       </c>
       <c r="H31">
-        <v>42015500</v>
+        <v>6999151</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
@@ -36024,7 +37578,7 @@
         <v>64</v>
       </c>
       <c r="H32">
-        <v>42368090</v>
+        <v>7845778</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -36053,7 +37607,7 @@
         <v>64</v>
       </c>
       <c r="H33">
-        <v>40427236</v>
+        <v>6750240</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -36082,7 +37636,7 @@
         <v>64</v>
       </c>
       <c r="H34">
-        <v>40252226</v>
+        <v>6457726</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -36111,7 +37665,7 @@
         <v>64</v>
       </c>
       <c r="H35">
-        <v>41133300</v>
+        <v>6818228</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -36140,7 +37694,7 @@
         <v>128</v>
       </c>
       <c r="H36">
-        <v>40729609</v>
+        <v>16550093</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -36169,7 +37723,7 @@
         <v>128</v>
       </c>
       <c r="H37">
-        <v>36483016</v>
+        <v>16350384</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -36198,7 +37752,7 @@
         <v>128</v>
       </c>
       <c r="H38">
-        <v>31855133</v>
+        <v>15994721</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -36227,7 +37781,7 @@
         <v>128</v>
       </c>
       <c r="H39">
-        <v>40721133</v>
+        <v>16195241</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -36256,7 +37810,7 @@
         <v>128</v>
       </c>
       <c r="H40">
-        <v>32243285</v>
+        <v>15902445</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -36285,7 +37839,7 @@
         <v>256</v>
       </c>
       <c r="H41">
-        <v>40473351</v>
+        <v>40663851</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -36314,7 +37868,7 @@
         <v>256</v>
       </c>
       <c r="H42">
-        <v>41033987</v>
+        <v>40443277</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -36343,7 +37897,7 @@
         <v>256</v>
       </c>
       <c r="H43">
-        <v>33582053</v>
+        <v>41961944</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -36372,7 +37926,7 @@
         <v>256</v>
       </c>
       <c r="H44">
-        <v>40948466</v>
+        <v>40447615</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -36401,7 +37955,7 @@
         <v>256</v>
       </c>
       <c r="H45">
-        <v>39618158</v>
+        <v>41489594</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -36430,7 +37984,7 @@
         <v>1</v>
       </c>
       <c r="H46">
-        <v>39165220</v>
+        <v>1260364</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -36459,7 +38013,7 @@
         <v>1</v>
       </c>
       <c r="H47">
-        <v>32688561</v>
+        <v>1285487</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -36488,7 +38042,7 @@
         <v>1</v>
       </c>
       <c r="H48">
-        <v>40754383</v>
+        <v>1245650</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -36517,7 +38071,7 @@
         <v>1</v>
       </c>
       <c r="H49">
-        <v>31678327</v>
+        <v>1246198</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -36546,7 +38100,7 @@
         <v>1</v>
       </c>
       <c r="H50">
-        <v>47686318</v>
+        <v>1240273</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -36575,7 +38129,7 @@
         <v>2</v>
       </c>
       <c r="H51">
-        <v>41706163</v>
+        <v>872682</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -36604,7 +38158,7 @@
         <v>2</v>
       </c>
       <c r="H52">
-        <v>40094197</v>
+        <v>885079</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -36633,7 +38187,7 @@
         <v>2</v>
       </c>
       <c r="H53">
-        <v>39774849</v>
+        <v>889398</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -36662,7 +38216,7 @@
         <v>2</v>
       </c>
       <c r="H54">
-        <v>40663626</v>
+        <v>909768</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -36691,7 +38245,7 @@
         <v>2</v>
       </c>
       <c r="H55">
-        <v>41365061</v>
+        <v>833340</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -36720,7 +38274,7 @@
         <v>4</v>
       </c>
       <c r="H56">
-        <v>47671503</v>
+        <v>765960</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -36749,7 +38303,7 @@
         <v>4</v>
       </c>
       <c r="H57">
-        <v>41512811</v>
+        <v>840541</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -36778,7 +38332,7 @@
         <v>4</v>
       </c>
       <c r="H58">
-        <v>41358155</v>
+        <v>862139</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -36807,7 +38361,7 @@
         <v>4</v>
       </c>
       <c r="H59">
-        <v>41706513</v>
+        <v>802234</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -36836,7 +38390,7 @@
         <v>4</v>
       </c>
       <c r="H60">
-        <v>40947124</v>
+        <v>738960</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -36865,7 +38419,7 @@
         <v>8</v>
       </c>
       <c r="H61">
-        <v>38772047</v>
+        <v>1053643</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -36894,7 +38448,7 @@
         <v>8</v>
       </c>
       <c r="H62">
-        <v>41428640</v>
+        <v>1053136</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -36923,7 +38477,7 @@
         <v>8</v>
       </c>
       <c r="H63">
-        <v>40438688</v>
+        <v>1042241</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -36952,7 +38506,7 @@
         <v>8</v>
       </c>
       <c r="H64">
-        <v>40440230</v>
+        <v>1037496</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -36981,7 +38535,7 @@
         <v>8</v>
       </c>
       <c r="H65">
-        <v>41296527</v>
+        <v>1077552</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -37010,7 +38564,7 @@
         <v>16</v>
       </c>
       <c r="H66">
-        <v>40770906</v>
+        <v>2617613</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -37039,7 +38593,7 @@
         <v>16</v>
       </c>
       <c r="H67">
-        <v>41410204</v>
+        <v>1828233</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -37068,7 +38622,7 @@
         <v>16</v>
       </c>
       <c r="H68">
-        <v>40305313</v>
+        <v>1805084</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -37097,7 +38651,7 @@
         <v>16</v>
       </c>
       <c r="H69">
-        <v>42340628</v>
+        <v>1860848</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -37126,7 +38680,7 @@
         <v>16</v>
       </c>
       <c r="H70">
-        <v>41149123</v>
+        <v>1730849</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -37155,7 +38709,7 @@
         <v>32</v>
       </c>
       <c r="H71">
-        <v>40142040</v>
+        <v>3388452</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -37184,7 +38738,7 @@
         <v>32</v>
       </c>
       <c r="H72">
-        <v>40875600</v>
+        <v>3626349</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -37213,7 +38767,7 @@
         <v>32</v>
       </c>
       <c r="H73">
-        <v>31876435</v>
+        <v>3620950</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -37242,7 +38796,7 @@
         <v>32</v>
       </c>
       <c r="H74">
-        <v>40399790</v>
+        <v>3503615</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -37271,7 +38825,7 @@
         <v>32</v>
       </c>
       <c r="H75">
-        <v>41759717</v>
+        <v>3590468</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -37300,7 +38854,7 @@
         <v>64</v>
       </c>
       <c r="H76">
-        <v>40026715</v>
+        <v>6738485</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -37329,7 +38883,7 @@
         <v>64</v>
       </c>
       <c r="H77">
-        <v>42038662</v>
+        <v>6898595</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -37358,7 +38912,7 @@
         <v>64</v>
       </c>
       <c r="H78">
-        <v>40392070</v>
+        <v>6650211</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -37387,7 +38941,7 @@
         <v>64</v>
       </c>
       <c r="H79">
-        <v>41937656</v>
+        <v>6872296</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -37416,7 +38970,7 @@
         <v>64</v>
       </c>
       <c r="H80">
-        <v>31165646</v>
+        <v>6905021</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -37445,7 +38999,7 @@
         <v>128</v>
       </c>
       <c r="H81">
-        <v>41352304</v>
+        <v>17053568</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -37474,7 +39028,7 @@
         <v>128</v>
       </c>
       <c r="H82">
-        <v>38989127</v>
+        <v>16457348</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -37503,7 +39057,7 @@
         <v>128</v>
       </c>
       <c r="H83">
-        <v>39984278</v>
+        <v>16298061</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
@@ -37532,7 +39086,7 @@
         <v>128</v>
       </c>
       <c r="H84">
-        <v>38558105</v>
+        <v>16076501</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -37561,7 +39115,7 @@
         <v>128</v>
       </c>
       <c r="H85">
-        <v>32305871</v>
+        <v>16019789</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
@@ -37590,7 +39144,7 @@
         <v>256</v>
       </c>
       <c r="H86">
-        <v>41175090</v>
+        <v>41754468</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
@@ -37619,7 +39173,7 @@
         <v>256</v>
       </c>
       <c r="H87">
-        <v>39774981</v>
+        <v>39790742</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -37648,7 +39202,7 @@
         <v>256</v>
       </c>
       <c r="H88">
-        <v>39809496</v>
+        <v>42562845</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
@@ -37677,7 +39231,7 @@
         <v>256</v>
       </c>
       <c r="H89">
-        <v>39411565</v>
+        <v>41174611</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
@@ -37706,7 +39260,7 @@
         <v>256</v>
       </c>
       <c r="H90">
-        <v>47464610</v>
+        <v>48578495</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
@@ -37735,7 +39289,7 @@
         <v>1</v>
       </c>
       <c r="H91">
-        <v>39770295</v>
+        <v>15489720</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -37764,7 +39318,7 @@
         <v>1</v>
       </c>
       <c r="H92">
-        <v>32611407</v>
+        <v>15860997</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
@@ -37793,7 +39347,7 @@
         <v>1</v>
       </c>
       <c r="H93">
-        <v>40234574</v>
+        <v>16117678</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -37822,7 +39376,7 @@
         <v>1</v>
       </c>
       <c r="H94">
-        <v>39983377</v>
+        <v>15573802</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
@@ -37851,7 +39405,7 @@
         <v>1</v>
       </c>
       <c r="H95">
-        <v>40162052</v>
+        <v>16201525</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
@@ -37880,7 +39434,7 @@
         <v>2</v>
       </c>
       <c r="H96">
-        <v>34869970</v>
+        <v>8640125</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
@@ -37909,7 +39463,7 @@
         <v>2</v>
       </c>
       <c r="H97">
-        <v>41503054</v>
+        <v>8582136</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
@@ -37938,7 +39492,7 @@
         <v>2</v>
       </c>
       <c r="H98">
-        <v>37856950</v>
+        <v>8299400</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
@@ -37967,7 +39521,7 @@
         <v>2</v>
       </c>
       <c r="H99">
-        <v>35843208</v>
+        <v>8281503</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
@@ -37996,7 +39550,7 @@
         <v>2</v>
       </c>
       <c r="H100">
-        <v>41548983</v>
+        <v>8458350</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
@@ -38025,7 +39579,7 @@
         <v>4</v>
       </c>
       <c r="H101">
-        <v>33209334</v>
+        <v>5354327</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
@@ -38054,7 +39608,7 @@
         <v>4</v>
       </c>
       <c r="H102">
-        <v>41565830</v>
+        <v>4879380</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
@@ -38083,7 +39637,7 @@
         <v>4</v>
       </c>
       <c r="H103">
-        <v>32950580</v>
+        <v>4736539</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
@@ -38112,7 +39666,7 @@
         <v>4</v>
       </c>
       <c r="H104">
-        <v>40508287</v>
+        <v>4947960</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
@@ -38141,7 +39695,7 @@
         <v>4</v>
       </c>
       <c r="H105">
-        <v>41536478</v>
+        <v>4951313</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
@@ -38170,7 +39724,7 @@
         <v>8</v>
       </c>
       <c r="H106">
-        <v>38970140</v>
+        <v>4672866</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
@@ -38199,7 +39753,7 @@
         <v>8</v>
       </c>
       <c r="H107">
-        <v>41699980</v>
+        <v>3343580</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
@@ -38228,7 +39782,7 @@
         <v>8</v>
       </c>
       <c r="H108">
-        <v>40531562</v>
+        <v>3582141</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
@@ -38257,7 +39811,7 @@
         <v>8</v>
       </c>
       <c r="H109">
-        <v>41026414</v>
+        <v>3408737</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
@@ -38286,7 +39840,7 @@
         <v>8</v>
       </c>
       <c r="H110">
-        <v>33407191</v>
+        <v>3588263</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
@@ -38315,7 +39869,7 @@
         <v>16</v>
       </c>
       <c r="H111">
-        <v>42413695</v>
+        <v>3746465</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
@@ -38344,7 +39898,7 @@
         <v>16</v>
       </c>
       <c r="H112">
-        <v>41939303</v>
+        <v>3692635</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
@@ -38373,7 +39927,7 @@
         <v>16</v>
       </c>
       <c r="H113">
-        <v>39064114</v>
+        <v>3439705</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
@@ -38402,7 +39956,7 @@
         <v>16</v>
       </c>
       <c r="H114">
-        <v>39964138</v>
+        <v>3361377</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
@@ -38431,7 +39985,7 @@
         <v>16</v>
       </c>
       <c r="H115">
-        <v>40672645</v>
+        <v>3393426</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
@@ -38460,7 +40014,7 @@
         <v>32</v>
       </c>
       <c r="H116">
-        <v>41570585</v>
+        <v>4885878</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
@@ -38489,7 +40043,7 @@
         <v>32</v>
       </c>
       <c r="H117">
-        <v>37002850</v>
+        <v>5027002</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
@@ -38518,7 +40072,7 @@
         <v>32</v>
       </c>
       <c r="H118">
-        <v>41346730</v>
+        <v>5061477</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
@@ -38547,7 +40101,7 @@
         <v>32</v>
       </c>
       <c r="H119">
-        <v>40225490</v>
+        <v>4980998</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
@@ -38576,7 +40130,7 @@
         <v>32</v>
       </c>
       <c r="H120">
-        <v>41035827</v>
+        <v>5205811</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -38605,7 +40159,7 @@
         <v>64</v>
       </c>
       <c r="H121">
-        <v>40470728</v>
+        <v>10434376</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
@@ -38634,7 +40188,7 @@
         <v>64</v>
       </c>
       <c r="H122">
-        <v>39821140</v>
+        <v>8108366</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
@@ -38663,7 +40217,7 @@
         <v>64</v>
       </c>
       <c r="H123">
-        <v>40222694</v>
+        <v>7935304</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
@@ -38692,7 +40246,7 @@
         <v>64</v>
       </c>
       <c r="H124">
-        <v>40463653</v>
+        <v>7917069</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
@@ -38721,7 +40275,7 @@
         <v>64</v>
       </c>
       <c r="H125">
-        <v>42407690</v>
+        <v>7782275</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
@@ -38750,7 +40304,7 @@
         <v>128</v>
       </c>
       <c r="H126">
-        <v>40753956</v>
+        <v>21428011</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
@@ -38779,7 +40333,7 @@
         <v>128</v>
       </c>
       <c r="H127">
-        <v>38971411</v>
+        <v>14720990</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
@@ -38808,7 +40362,7 @@
         <v>128</v>
       </c>
       <c r="H128">
-        <v>40831015</v>
+        <v>14851480</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
@@ -38837,7 +40391,7 @@
         <v>128</v>
       </c>
       <c r="H129">
-        <v>39662343</v>
+        <v>14923675</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
@@ -38866,7 +40420,7 @@
         <v>128</v>
       </c>
       <c r="H130">
-        <v>40889743</v>
+        <v>16813359</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
@@ -38895,7 +40449,7 @@
         <v>256</v>
       </c>
       <c r="H131">
-        <v>40113861</v>
+        <v>40517988</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
@@ -38924,7 +40478,7 @@
         <v>256</v>
       </c>
       <c r="H132">
-        <v>41287634</v>
+        <v>40249894</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
@@ -38953,7 +40507,7 @@
         <v>256</v>
       </c>
       <c r="H133">
-        <v>42809568</v>
+        <v>35924498</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
@@ -38982,7 +40536,7 @@
         <v>256</v>
       </c>
       <c r="H134">
-        <v>39907289</v>
+        <v>32981657</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
@@ -39011,7 +40565,7 @@
         <v>256</v>
       </c>
       <c r="H135">
-        <v>40710190</v>
+        <v>38404883</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
@@ -39040,7 +40594,7 @@
         <v>1</v>
       </c>
       <c r="H136">
-        <v>42117745</v>
+        <v>232734600</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
@@ -39069,7 +40623,7 @@
         <v>1</v>
       </c>
       <c r="H137">
-        <v>44885760</v>
+        <v>232734600</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
@@ -39098,7 +40652,7 @@
         <v>1</v>
       </c>
       <c r="H138">
-        <v>42117745</v>
+        <v>232734600</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
@@ -39127,7 +40681,7 @@
         <v>1</v>
       </c>
       <c r="H139">
-        <v>42117745</v>
+        <v>232734600</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
@@ -39156,7 +40710,7 @@
         <v>1</v>
       </c>
       <c r="H140">
-        <v>42117745</v>
+        <v>232734600</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
@@ -39185,7 +40739,7 @@
         <v>2</v>
       </c>
       <c r="H141">
-        <v>42967557</v>
+        <v>117073244</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
@@ -39214,7 +40768,7 @@
         <v>2</v>
       </c>
       <c r="H142">
-        <v>42967557</v>
+        <v>117073244</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
@@ -39243,7 +40797,7 @@
         <v>2</v>
       </c>
       <c r="H143">
-        <v>42967557</v>
+        <v>117073244</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
@@ -39272,7 +40826,7 @@
         <v>2</v>
       </c>
       <c r="H144">
-        <v>42967557</v>
+        <v>117073244</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
@@ -39301,7 +40855,7 @@
         <v>2</v>
       </c>
       <c r="H145">
-        <v>42967557</v>
+        <v>117073244</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
@@ -39330,7 +40884,7 @@
         <v>4</v>
       </c>
       <c r="H146">
-        <v>42993044</v>
+        <v>59039410</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
@@ -39359,7 +40913,7 @@
         <v>4</v>
       </c>
       <c r="H147">
-        <v>42993044</v>
+        <v>59039410</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
@@ -39388,7 +40942,7 @@
         <v>4</v>
       </c>
       <c r="H148">
-        <v>42993044</v>
+        <v>59039410</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
@@ -39417,7 +40971,7 @@
         <v>4</v>
       </c>
       <c r="H149">
-        <v>42993044</v>
+        <v>59039410</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
@@ -39446,7 +41000,7 @@
         <v>4</v>
       </c>
       <c r="H150">
-        <v>42993044</v>
+        <v>59039410</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
@@ -39475,7 +41029,7 @@
         <v>8</v>
       </c>
       <c r="H151">
-        <v>43006088</v>
+        <v>30564546</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
@@ -39504,7 +41058,7 @@
         <v>8</v>
       </c>
       <c r="H152">
-        <v>43006088</v>
+        <v>30564546</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
@@ -39533,7 +41087,7 @@
         <v>8</v>
       </c>
       <c r="H153">
-        <v>43006088</v>
+        <v>30564546</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
@@ -39562,7 +41116,7 @@
         <v>8</v>
       </c>
       <c r="H154">
-        <v>43006088</v>
+        <v>30564546</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
@@ -39591,7 +41145,7 @@
         <v>8</v>
       </c>
       <c r="H155">
-        <v>43006088</v>
+        <v>30564546</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
@@ -39620,7 +41174,7 @@
         <v>16</v>
       </c>
       <c r="H156">
-        <v>42381439</v>
+        <v>17148164</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
@@ -39649,7 +41203,7 @@
         <v>16</v>
       </c>
       <c r="H157">
-        <v>42381439</v>
+        <v>17148164</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
@@ -39678,7 +41232,7 @@
         <v>16</v>
       </c>
       <c r="H158">
-        <v>42381439</v>
+        <v>17148164</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
@@ -39707,7 +41261,7 @@
         <v>16</v>
       </c>
       <c r="H159">
-        <v>42381439</v>
+        <v>17148164</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
@@ -39736,7 +41290,7 @@
         <v>16</v>
       </c>
       <c r="H160">
-        <v>42381439</v>
+        <v>17148164</v>
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.25">
@@ -39765,7 +41319,7 @@
         <v>32</v>
       </c>
       <c r="H161">
-        <v>43585675</v>
+        <v>16790151</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
@@ -39794,7 +41348,7 @@
         <v>32</v>
       </c>
       <c r="H162">
-        <v>43585675</v>
+        <v>16790151</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.25">
@@ -39823,7 +41377,7 @@
         <v>32</v>
       </c>
       <c r="H163">
-        <v>43585675</v>
+        <v>16790151</v>
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.25">
@@ -39852,7 +41406,7 @@
         <v>32</v>
       </c>
       <c r="H164">
-        <v>43585675</v>
+        <v>16790151</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.25">
@@ -39881,7 +41435,7 @@
         <v>32</v>
       </c>
       <c r="H165">
-        <v>43585675</v>
+        <v>16790151</v>
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.25">
@@ -39910,7 +41464,7 @@
         <v>64</v>
       </c>
       <c r="H166">
-        <v>41222973</v>
+        <v>18761012</v>
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.25">
@@ -39939,7 +41493,7 @@
         <v>64</v>
       </c>
       <c r="H167">
-        <v>41222973</v>
+        <v>18761012</v>
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.25">
@@ -39968,7 +41522,7 @@
         <v>64</v>
       </c>
       <c r="H168">
-        <v>41222973</v>
+        <v>18761012</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.25">
@@ -39997,7 +41551,7 @@
         <v>64</v>
       </c>
       <c r="H169">
-        <v>41222973</v>
+        <v>18761012</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.25">
@@ -40026,7 +41580,7 @@
         <v>64</v>
       </c>
       <c r="H170">
-        <v>41222973</v>
+        <v>18761012</v>
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.25">
@@ -40055,11 +41609,11 @@
         <v>128</v>
       </c>
       <c r="H171">
-        <v>42540816</v>
+        <v>27205123</v>
       </c>
       <c r="I171">
         <f>MIN(H171:H175)</f>
-        <v>42540816</v>
+        <v>27205123</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
@@ -40088,7 +41642,7 @@
         <v>128</v>
       </c>
       <c r="H172">
-        <v>42540816</v>
+        <v>27205123</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
@@ -40117,7 +41671,7 @@
         <v>128</v>
       </c>
       <c r="H173">
-        <v>42540816</v>
+        <v>27205123</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.25">
@@ -40146,7 +41700,7 @@
         <v>128</v>
       </c>
       <c r="H174">
-        <v>42540816</v>
+        <v>27205123</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
@@ -40175,7 +41729,7 @@
         <v>128</v>
       </c>
       <c r="H175">
-        <v>42540816</v>
+        <v>27205123</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.25">
@@ -40204,11 +41758,11 @@
         <v>256</v>
       </c>
       <c r="H176">
-        <v>42031710</v>
+        <v>50578079</v>
       </c>
       <c r="I176">
         <f>MIN(H176:H180)</f>
-        <v>42031710</v>
+        <v>50578079</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.25">
@@ -40237,7 +41791,7 @@
         <v>256</v>
       </c>
       <c r="H177">
-        <v>42031710</v>
+        <v>50578079</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.25">
@@ -40266,7 +41820,7 @@
         <v>256</v>
       </c>
       <c r="H178">
-        <v>42031710</v>
+        <v>50578079</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.25">
@@ -40295,7 +41849,7 @@
         <v>256</v>
       </c>
       <c r="H179">
-        <v>42031710</v>
+        <v>50578079</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.25">
@@ -40324,7 +41878,7 @@
         <v>256</v>
       </c>
       <c r="H180">
-        <v>42031710</v>
+        <v>50578079</v>
       </c>
     </row>
   </sheetData>

</xml_diff>